<commit_message>
Updated code for final report
Updates with fixes
</commit_message>
<xml_diff>
--- a/hCREiAM_IPC_Parameters.xlsx
+++ b/hCREiAM_IPC_Parameters.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cddepadmin/Documents/IPC HAI CRE Project Code/IPC Model on AWS/September 10th Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cddepadmin/Documents/IPC HAI CRE Project Code/HospitalCREInterventionAssessmentModel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E7B241-779B-6D41-8705-22D60E26A834}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED764E9-FB35-294A-BB0C-88E8398B7541}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="2260" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline" sheetId="3" r:id="rId1"/>
     <sheet name="Interventions" sheetId="5" r:id="rId2"/>
+    <sheet name="HealthCareFacility" sheetId="6" r:id="rId3"/>
+    <sheet name="Cost" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="165">
   <si>
     <t>pi.lhs</t>
   </si>
@@ -329,16 +331,228 @@
   </si>
   <si>
     <t>tau.1</t>
+  </si>
+  <si>
+    <t>High Environmental Transmission</t>
+  </si>
+  <si>
+    <t>triangle</t>
+  </si>
+  <si>
+    <t>ICOrder</t>
+  </si>
+  <si>
+    <t>qnp</t>
+  </si>
+  <si>
+    <t>aS.1</t>
+  </si>
+  <si>
+    <t>aS.2</t>
+  </si>
+  <si>
+    <t>rn.1</t>
+  </si>
+  <si>
+    <t>rn.2</t>
+  </si>
+  <si>
+    <t>rd.1</t>
+  </si>
+  <si>
+    <t>rd.2</t>
+  </si>
+  <si>
+    <t>S.1</t>
+  </si>
+  <si>
+    <t>S.2</t>
+  </si>
+  <si>
+    <t>Number of Runs</t>
+  </si>
+  <si>
+    <t>HET_IN</t>
+  </si>
+  <si>
+    <t>LET_IN</t>
+  </si>
+  <si>
+    <t>HET_SA</t>
+  </si>
+  <si>
+    <t>LET_SA</t>
+  </si>
+  <si>
+    <t>qdp</t>
+  </si>
+  <si>
+    <t># Environmental Transmission Rate</t>
+  </si>
+  <si>
+    <t># Low Environmental Transmission</t>
+  </si>
+  <si>
+    <t># India Health Center</t>
+  </si>
+  <si>
+    <t># South Africa Health Center</t>
+  </si>
+  <si>
+    <t>numbeds</t>
+  </si>
+  <si>
+    <t>India HET</t>
+  </si>
+  <si>
+    <t>India LET</t>
+  </si>
+  <si>
+    <t>South Africa HET</t>
+  </si>
+  <si>
+    <t>South Africa LET</t>
+  </si>
+  <si>
+    <t>ICUASJU</t>
+  </si>
+  <si>
+    <t>ICUASCPCHG</t>
+  </si>
+  <si>
+    <t># ICU Only Active Surveillance</t>
+  </si>
+  <si>
+    <t>PS.ICU.1</t>
+  </si>
+  <si>
+    <t>PS.ICU.2</t>
+  </si>
+  <si>
+    <t>OM.ICU.1</t>
+  </si>
+  <si>
+    <t>OM.ICU.2</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>CP.cost</t>
+  </si>
+  <si>
+    <t>CHG.cost</t>
+  </si>
+  <si>
+    <t>ASCPCHG.cost</t>
+  </si>
+  <si>
+    <t>ICUASCPCHG.cost</t>
+  </si>
+  <si>
+    <t>HH.cost</t>
+  </si>
+  <si>
+    <t>EC4.cost</t>
+  </si>
+  <si>
+    <t>JU.cost</t>
+  </si>
+  <si>
+    <t>ASJU.cost</t>
+  </si>
+  <si>
+    <t>ICUASJU.cost</t>
+  </si>
+  <si>
+    <t>ASCHRT.cost</t>
+  </si>
+  <si>
+    <t>CHRT.cost</t>
+  </si>
+  <si>
+    <t>ALL.cost</t>
+  </si>
+  <si>
+    <t># High Environmental Transmsission in South Africa</t>
+  </si>
+  <si>
+    <t># High Environmental Transmsission in India</t>
+  </si>
+  <si>
+    <t># Low Environmental Transmsission in South Africa</t>
+  </si>
+  <si>
+    <t># Low Environmental Transmsission in India</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>CHRT</t>
+  </si>
+  <si>
+    <t>ASCHRT</t>
+  </si>
+  <si>
+    <t># Cohorting</t>
+  </si>
+  <si>
+    <t>f.1</t>
+  </si>
+  <si>
+    <t>f.2</t>
+  </si>
+  <si>
+    <t>Fn.1</t>
+  </si>
+  <si>
+    <t>Fn.2</t>
+  </si>
+  <si>
+    <t>distribution</t>
+  </si>
+  <si>
+    <t>triangular</t>
+  </si>
+  <si>
+    <t>Cost of Intervention</t>
+  </si>
+  <si>
+    <t>CostPerInf.GW</t>
+  </si>
+  <si>
+    <t>CostPerInf.ICU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -364,12 +578,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -690,7 +907,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1434,10 +1651,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q59"/>
+  <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58:G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1453,20 +1670,20 @@
     <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1498,33 +1715,45 @@
         <v>89</v>
       </c>
       <c r="K2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" t="s">
+        <v>127</v>
+      </c>
+      <c r="M2" t="s">
         <v>91</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>92</v>
       </c>
-      <c r="M2" t="s">
-        <v>90</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>93</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q2" t="s">
         <v>94</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>95</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
+        <v>153</v>
+      </c>
+      <c r="T2" t="s">
+        <v>154</v>
+      </c>
+      <c r="U2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1549,14 +1778,17 @@
       <c r="J4">
         <v>1</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1581,24 +1813,27 @@
       <c r="J5">
         <v>1</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1620,17 +1855,20 @@
       <c r="G8">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -1652,17 +1890,20 @@
       <c r="G9" s="2">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1684,17 +1925,20 @@
       <c r="G10">
         <v>0.09</v>
       </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="Q10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -1716,407 +1960,383 @@
       <c r="G11">
         <v>0.09</v>
       </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="Q11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f>1/14</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="F17">
+        <f>3/14</f>
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="G17">
+        <f>1/7</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>51</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
         <v>0.25</v>
       </c>
-      <c r="F14">
+      <c r="F20">
         <v>0.75</v>
       </c>
-      <c r="G14">
+      <c r="G20">
         <v>0.5</v>
       </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="Q14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>52</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
         <v>0.25</v>
       </c>
-      <c r="F15">
+      <c r="F21">
         <v>0.75</v>
       </c>
-      <c r="G15">
+      <c r="G21">
         <v>0.5</v>
       </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="Q15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>53</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
         <v>2</v>
       </c>
-      <c r="F18">
+      <c r="F24">
         <v>3</v>
       </c>
-      <c r="G18">
+      <c r="G24">
         <f xml:space="preserve"> 5/2</f>
         <v>2.5</v>
       </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-      <c r="Q18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="U24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>54</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
         <v>2</v>
       </c>
-      <c r="F19">
+      <c r="F25">
         <v>3</v>
       </c>
-      <c r="G19">
-        <f t="shared" ref="G19:G21" si="0" xml:space="preserve"> 5/2</f>
+      <c r="G25">
+        <f t="shared" ref="G25:G27" si="0" xml:space="preserve"> 5/2</f>
         <v>2.5</v>
       </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="Q19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>55</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
         <v>2</v>
       </c>
-      <c r="F20">
+      <c r="F26">
         <v>3</v>
       </c>
-      <c r="G20">
+      <c r="G26">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="Q20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="U26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>56</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
         <v>2</v>
       </c>
-      <c r="F21">
+      <c r="F27">
         <v>3</v>
       </c>
-      <c r="G21">
+      <c r="G27">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="U27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>57</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0.26400000000000001</v>
-      </c>
-      <c r="F24">
-        <v>1.032</v>
-      </c>
-      <c r="G24">
-        <v>0.58799999999999997</v>
-      </c>
-      <c r="O24">
-        <v>1</v>
-      </c>
-      <c r="Q24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0.26400000000000001</v>
-      </c>
-      <c r="F25">
-        <v>1.032</v>
-      </c>
-      <c r="G25">
-        <v>0.58799999999999997</v>
-      </c>
-      <c r="O25">
-        <v>1</v>
-      </c>
-      <c r="Q25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0.92</v>
-      </c>
-      <c r="F26">
-        <v>1.6279999999999999</v>
-      </c>
-      <c r="G26">
-        <v>1.274</v>
-      </c>
-      <c r="O26">
-        <v>1</v>
-      </c>
-      <c r="Q26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0.92</v>
-      </c>
-      <c r="F27">
-        <v>1.6279999999999999</v>
-      </c>
-      <c r="G27">
-        <v>1.274</v>
-      </c>
-      <c r="O27">
-        <v>1</v>
-      </c>
-      <c r="Q27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="F28">
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="G28">
-        <v>0.29399999999999998</v>
-      </c>
-      <c r="O28">
-        <v>1</v>
-      </c>
-      <c r="Q28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="F29">
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="G29">
-        <v>0.29399999999999998</v>
-      </c>
-      <c r="O29">
-        <v>1</v>
-      </c>
-      <c r="Q29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>63</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -2136,16 +2356,16 @@
       <c r="G30">
         <v>0.58799999999999997</v>
       </c>
-      <c r="P30">
-        <v>1</v>
-      </c>
       <c r="Q30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="U30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -2165,564 +2385,707 @@
       <c r="G31">
         <v>0.58799999999999997</v>
       </c>
-      <c r="P31">
-        <v>1</v>
-      </c>
       <c r="Q31">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="U31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0.92</v>
+      </c>
+      <c r="F32">
+        <v>1.6279999999999999</v>
+      </c>
+      <c r="G32">
+        <v>1.274</v>
+      </c>
+      <c r="Q32">
+        <v>1</v>
+      </c>
+      <c r="U32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0.92</v>
+      </c>
+      <c r="F33">
+        <v>1.6279999999999999</v>
+      </c>
+      <c r="G33">
+        <v>1.274</v>
+      </c>
+      <c r="Q33">
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="F34">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="G34">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="Q34">
+        <v>1</v>
+      </c>
+      <c r="U34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="F35">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="G35">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
+      </c>
+      <c r="U35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="F36">
+        <v>1.032</v>
+      </c>
+      <c r="G36">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="R36">
+        <v>1</v>
+      </c>
+      <c r="U36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="F37">
+        <v>1.032</v>
+      </c>
+      <c r="G37">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="R37">
+        <v>1</v>
+      </c>
+      <c r="U37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>65</v>
       </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
         <v>0.83599999999999997</v>
       </c>
-      <c r="F33">
+      <c r="F39">
         <v>2.3199999999999998</v>
       </c>
-      <c r="G33">
+      <c r="G39">
         <v>1.5960000000000001</v>
       </c>
-      <c r="O33">
-        <v>1</v>
-      </c>
-      <c r="Q33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="Q39">
+        <v>1</v>
+      </c>
+      <c r="U39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>66</v>
       </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
         <v>0.83599999999999997</v>
       </c>
-      <c r="F34">
+      <c r="F40">
         <v>2.3199999999999998</v>
       </c>
-      <c r="G34">
+      <c r="G40">
         <v>1.5960000000000001</v>
       </c>
-      <c r="O34">
-        <v>1</v>
-      </c>
-      <c r="Q34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="Q40">
+        <v>1</v>
+      </c>
+      <c r="U40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>67</v>
       </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
         <v>0.41799999999999998</v>
       </c>
-      <c r="F35">
+      <c r="F41">
         <v>1.1599999999999999</v>
       </c>
-      <c r="G35">
+      <c r="G41">
         <v>0.79800000000000004</v>
       </c>
-      <c r="O35">
-        <v>1</v>
-      </c>
-      <c r="Q35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="Q41">
+        <v>1</v>
+      </c>
+      <c r="U41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>68</v>
       </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
         <v>0.41799999999999998</v>
       </c>
-      <c r="F36">
+      <c r="F42">
         <v>1.1599999999999999</v>
       </c>
-      <c r="G36">
+      <c r="G42">
         <v>0.79800000000000004</v>
       </c>
-      <c r="O36">
-        <v>1</v>
-      </c>
-      <c r="Q36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="Q42">
+        <v>1</v>
+      </c>
+      <c r="U42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>69</v>
       </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
         <v>0.20799999999999999</v>
       </c>
-      <c r="F37">
+      <c r="F43">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G37">
+      <c r="G43">
         <v>0.39800000000000002</v>
       </c>
-      <c r="O37">
-        <v>1</v>
-      </c>
-      <c r="Q37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="Q43">
+        <v>1</v>
+      </c>
+      <c r="U43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>70</v>
       </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
         <v>0.20799999999999999</v>
       </c>
-      <c r="F38">
+      <c r="F44">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G38">
+      <c r="G44">
         <v>0.39800000000000002</v>
       </c>
-      <c r="O38">
-        <v>1</v>
-      </c>
-      <c r="Q38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="Q44">
+        <v>1</v>
+      </c>
+      <c r="U44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>71</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41">
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
         <v>0.45</v>
       </c>
-      <c r="F41">
+      <c r="F47">
         <v>0.75</v>
       </c>
-      <c r="G41">
+      <c r="G47">
         <v>0.6</v>
       </c>
-      <c r="L41">
-        <v>1</v>
-      </c>
-      <c r="N41">
-        <v>1</v>
-      </c>
-      <c r="Q41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="P47">
+        <v>1</v>
+      </c>
+      <c r="U47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>72</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42">
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
         <v>0.45</v>
       </c>
-      <c r="F42">
+      <c r="F48">
         <v>0.75</v>
       </c>
-      <c r="G42">
+      <c r="G48">
         <v>0.6</v>
       </c>
-      <c r="L42">
-        <v>1</v>
-      </c>
-      <c r="N42">
-        <v>1</v>
-      </c>
-      <c r="Q42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="N48">
+        <v>1</v>
+      </c>
+      <c r="O48">
+        <v>1</v>
+      </c>
+      <c r="P48">
+        <v>1</v>
+      </c>
+      <c r="U48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>73</v>
       </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43">
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
         <v>1.5</v>
       </c>
-      <c r="G43">
+      <c r="G49">
         <v>1.2</v>
       </c>
-      <c r="L43">
-        <v>1</v>
-      </c>
-      <c r="N43">
-        <v>1</v>
-      </c>
-      <c r="Q43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="N49">
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
+      <c r="P49">
+        <v>1</v>
+      </c>
+      <c r="U49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>74</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-      <c r="F44">
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
         <v>1.5</v>
       </c>
-      <c r="G44">
+      <c r="G50">
         <v>1.2</v>
       </c>
-      <c r="L44">
-        <v>1</v>
-      </c>
-      <c r="N44">
-        <v>1</v>
-      </c>
-      <c r="Q44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="N50">
+        <v>1</v>
+      </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="P50">
+        <v>1</v>
+      </c>
+      <c r="U50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>75</v>
       </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-      <c r="F45">
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
         <v>1.5</v>
       </c>
-      <c r="G45">
+      <c r="G51">
         <v>1.18</v>
       </c>
-      <c r="L45">
-        <v>1</v>
-      </c>
-      <c r="N45">
-        <v>1</v>
-      </c>
-      <c r="Q45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="N51">
+        <v>1</v>
+      </c>
+      <c r="O51">
+        <v>1</v>
+      </c>
+      <c r="P51">
+        <v>1</v>
+      </c>
+      <c r="U51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>76</v>
       </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46">
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
         <v>1.5</v>
       </c>
-      <c r="G46">
+      <c r="G52">
         <v>1.18</v>
       </c>
-      <c r="L46">
-        <v>1</v>
-      </c>
-      <c r="N46">
-        <v>1</v>
-      </c>
-      <c r="Q46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>22</v>
-      </c>
-      <c r="C53">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="D53">
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="E53">
-        <v>0.29399999999999998</v>
-      </c>
-      <c r="F53">
-        <f>3*C53</f>
-        <v>0.39600000000000002</v>
-      </c>
-      <c r="G53">
-        <f t="shared" ref="G53:H53" si="1">3*D53</f>
-        <v>1.548</v>
-      </c>
-      <c r="H53">
-        <f t="shared" si="1"/>
-        <v>0.8819999999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
-        <v>23</v>
-      </c>
-      <c r="C54">
-        <v>0.46</v>
-      </c>
-      <c r="D54">
-        <v>0.81399999999999995</v>
-      </c>
-      <c r="E54">
-        <v>0.63700000000000001</v>
-      </c>
-      <c r="F54">
-        <f t="shared" ref="F54:F59" si="2">3*C54</f>
-        <v>1.3800000000000001</v>
-      </c>
-      <c r="G54">
-        <f t="shared" ref="G54:G59" si="3">3*D54</f>
-        <v>2.4419999999999997</v>
-      </c>
-      <c r="H54">
-        <f t="shared" ref="H54:H59" si="4">3*E54</f>
-        <v>1.911</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
-        <v>24</v>
+      <c r="N52">
+        <v>1</v>
+      </c>
+      <c r="O52">
+        <v>1</v>
+      </c>
+      <c r="P52">
+        <v>1</v>
+      </c>
+      <c r="U52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>156</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
       </c>
       <c r="C55">
-        <v>0.41799999999999998</v>
+        <v>1</v>
       </c>
       <c r="D55">
-        <v>1.1599999999999999</v>
+        <v>1</v>
       </c>
       <c r="E55">
-        <v>0.79800000000000004</v>
+        <v>0.98</v>
       </c>
       <c r="F55">
-        <f t="shared" si="2"/>
-        <v>1.254</v>
+        <v>1</v>
       </c>
       <c r="G55">
-        <f t="shared" si="3"/>
-        <v>3.4799999999999995</v>
-      </c>
-      <c r="H55">
-        <f t="shared" si="4"/>
-        <v>2.3940000000000001</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
-        <v>25</v>
+        <v>0.99</v>
+      </c>
+      <c r="S55">
+        <v>1</v>
+      </c>
+      <c r="T55">
+        <v>1</v>
+      </c>
+      <c r="U55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>157</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
       </c>
       <c r="C56">
-        <v>0.20899999999999999</v>
+        <v>1</v>
       </c>
       <c r="D56">
-        <v>0.57999999999999996</v>
+        <v>1</v>
       </c>
       <c r="E56">
-        <v>0.39900000000000002</v>
+        <v>0.98</v>
       </c>
       <c r="F56">
-        <f t="shared" si="2"/>
-        <v>0.627</v>
+        <v>1</v>
       </c>
       <c r="G56">
-        <f t="shared" si="3"/>
-        <v>1.7399999999999998</v>
-      </c>
-      <c r="H56">
-        <f t="shared" si="4"/>
-        <v>1.1970000000000001</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>26</v>
+        <v>0.99</v>
+      </c>
+      <c r="S56">
+        <v>1</v>
+      </c>
+      <c r="T56">
+        <v>1</v>
+      </c>
+      <c r="U56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>158</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
       </c>
       <c r="C57">
-        <v>0.104</v>
+        <v>1</v>
       </c>
       <c r="D57">
-        <v>0.28999999999999998</v>
+        <v>1</v>
       </c>
       <c r="E57">
-        <v>0.19900000000000001</v>
+        <v>0.98</v>
       </c>
       <c r="F57">
-        <f t="shared" si="2"/>
-        <v>0.312</v>
+        <v>1</v>
       </c>
       <c r="G57">
-        <f t="shared" si="3"/>
-        <v>0.86999999999999988</v>
-      </c>
-      <c r="H57">
-        <f t="shared" si="4"/>
-        <v>0.59699999999999998</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
-        <v>27</v>
+        <v>0.99</v>
+      </c>
+      <c r="S57">
+        <v>1</v>
+      </c>
+      <c r="T57">
+        <v>1</v>
+      </c>
+      <c r="U57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>159</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>2.1999999999999999E-2</v>
+        <v>1</v>
       </c>
       <c r="D58">
-        <v>0.09</v>
+        <v>1</v>
       </c>
       <c r="E58">
-        <v>4.9000000000000002E-2</v>
+        <v>0.98</v>
       </c>
       <c r="F58">
-        <f t="shared" si="2"/>
-        <v>6.6000000000000003E-2</v>
+        <v>1</v>
       </c>
       <c r="G58">
-        <f t="shared" si="3"/>
-        <v>0.27</v>
-      </c>
-      <c r="H58">
-        <f t="shared" si="4"/>
-        <v>0.14700000000000002</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
-        <v>28</v>
-      </c>
-      <c r="C59">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="D59">
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="E59">
-        <v>0.29399999999999998</v>
-      </c>
-      <c r="F59">
-        <f t="shared" si="2"/>
-        <v>0.39600000000000002</v>
-      </c>
-      <c r="G59">
-        <f t="shared" si="3"/>
-        <v>1.548</v>
-      </c>
-      <c r="H59">
-        <f t="shared" si="4"/>
-        <v>0.8819999999999999</v>
+        <v>0.99</v>
+      </c>
+      <c r="S58">
+        <v>1</v>
+      </c>
+      <c r="T58">
+        <v>1</v>
+      </c>
+      <c r="U58">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2732,4 +3095,1889 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11750CF3-3AEA-5043-93F2-0A2DC2BCA1C1}">
+  <dimension ref="A1:J40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4">
+        <v>1E-4</v>
+      </c>
+      <c r="C4">
+        <v>4.6000000000000001E-4</v>
+      </c>
+      <c r="D4">
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5">
+        <v>1E-4</v>
+      </c>
+      <c r="C5">
+        <v>4.6000000000000001E-4</v>
+      </c>
+      <c r="D5">
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C9">
+        <v>1.1199999999999999E-3</v>
+      </c>
+      <c r="D9">
+        <v>5.5999999999999995E-4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C10">
+        <v>1.1199999999999999E-3</v>
+      </c>
+      <c r="D10">
+        <v>5.5999999999999995E-4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14">
+        <v>392</v>
+      </c>
+      <c r="C14">
+        <v>392</v>
+      </c>
+      <c r="D14">
+        <v>392</v>
+      </c>
+      <c r="E14" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15">
+        <f>343/392</f>
+        <v>0.875</v>
+      </c>
+      <c r="C15">
+        <f>343/392</f>
+        <v>0.875</v>
+      </c>
+      <c r="D15">
+        <f>343/392</f>
+        <v>0.875</v>
+      </c>
+      <c r="E15" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16">
+        <f>49/392</f>
+        <v>0.125</v>
+      </c>
+      <c r="C16">
+        <f>49/392</f>
+        <v>0.125</v>
+      </c>
+      <c r="D16">
+        <f>49/392</f>
+        <v>0.125</v>
+      </c>
+      <c r="E16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18">
+        <v>0.45</v>
+      </c>
+      <c r="C18">
+        <v>0.75</v>
+      </c>
+      <c r="D18">
+        <v>0.6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>100</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19">
+        <v>0.45</v>
+      </c>
+      <c r="C19">
+        <v>0.75</v>
+      </c>
+      <c r="D19">
+        <v>0.6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>6.19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>100</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1.8</v>
+      </c>
+      <c r="D22">
+        <v>1.4219999999999999</v>
+      </c>
+      <c r="E22" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <v>12.51</v>
+      </c>
+      <c r="E23" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C24">
+        <v>3.5</v>
+      </c>
+      <c r="D24">
+        <v>2.91</v>
+      </c>
+      <c r="E24" t="s">
+        <v>100</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27">
+        <v>324</v>
+      </c>
+      <c r="C27">
+        <v>324</v>
+      </c>
+      <c r="D27">
+        <v>324</v>
+      </c>
+      <c r="E27" t="s">
+        <v>100</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28">
+        <f>307/324</f>
+        <v>0.94753086419753085</v>
+      </c>
+      <c r="C28">
+        <f>307/324</f>
+        <v>0.94753086419753085</v>
+      </c>
+      <c r="D28">
+        <f>307/324</f>
+        <v>0.94753086419753085</v>
+      </c>
+      <c r="E28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29">
+        <f>17/324</f>
+        <v>5.2469135802469133E-2</v>
+      </c>
+      <c r="C29">
+        <f>17/324</f>
+        <v>5.2469135802469133E-2</v>
+      </c>
+      <c r="D29">
+        <f>17/324</f>
+        <v>5.2469135802469133E-2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>100</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31">
+        <v>0.9</v>
+      </c>
+      <c r="C31">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D31">
+        <v>0.95</v>
+      </c>
+      <c r="E31" t="s">
+        <v>100</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32">
+        <v>0.9</v>
+      </c>
+      <c r="C32">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D32">
+        <v>0.95</v>
+      </c>
+      <c r="E32" t="s">
+        <v>100</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <v>4.04</v>
+      </c>
+      <c r="E34" t="s">
+        <v>100</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="C35">
+        <v>1.333</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>100</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36">
+        <v>5.62</v>
+      </c>
+      <c r="C36">
+        <v>9</v>
+      </c>
+      <c r="D36">
+        <v>7.31</v>
+      </c>
+      <c r="E36" t="s">
+        <v>100</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37">
+        <v>1.5</v>
+      </c>
+      <c r="C37">
+        <v>2.5</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>100</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40">
+        <v>365</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD6C287A-A914-2441-8520-643919F438F4}">
+  <dimension ref="A1:I63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="3">
+        <v>372739.43022844777</v>
+      </c>
+      <c r="C3" s="3">
+        <v>452396.13707112777</v>
+      </c>
+      <c r="D3" s="3">
+        <v>412567.78364978777</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="3">
+        <v>116618.35407504012</v>
+      </c>
+      <c r="C4" s="3">
+        <v>131597.41260746546</v>
+      </c>
+      <c r="D4" s="3">
+        <v>124107.88334125279</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="3">
+        <v>6046151.8518112488</v>
+      </c>
+      <c r="C5" s="3">
+        <v>7422005.7661387259</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6734078.8089749869</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2580376.102621302</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3057908.3557115062</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2819142.2291664043</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="3">
+        <v>412003.92714285717</v>
+      </c>
+      <c r="C7" s="3">
+        <v>993370.92714285711</v>
+      </c>
+      <c r="D7" s="3">
+        <v>679905.92714285711</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2121892.0299567101</v>
+      </c>
+      <c r="C8" s="3">
+        <v>4828497.67995671</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2979969.0299567101</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1224606.7557142859</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4476294.0835714294</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3045723.5235714288</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="3">
+        <v>5699364.7241007974</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10326905.966285417</v>
+      </c>
+      <c r="D10" s="3">
+        <v>8208408.4491216782</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2962518.6551757222</v>
+      </c>
+      <c r="C11" s="3">
+        <v>6691738.2361230711</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5022401.5495779682</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="3">
+        <v>5586909.0526265362</v>
+      </c>
+      <c r="C12" s="3">
+        <v>7132225.5232976777</v>
+      </c>
+      <c r="D12" s="3">
+        <v>6359567.2879621061</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" s="3">
+        <v>630584.52044832578</v>
+      </c>
+      <c r="C13" s="3">
+        <v>711818.5262609612</v>
+      </c>
+      <c r="D13" s="3">
+        <v>671201.52335464349</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="3">
+        <v>10435239.085073428</v>
+      </c>
+      <c r="C14" s="3">
+        <v>18431986.983070683</v>
+      </c>
+      <c r="D14" s="3">
+        <v>14110878.813000625</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="3">
+        <v>9381</v>
+      </c>
+      <c r="C15" s="3">
+        <v>23884</v>
+      </c>
+      <c r="D15" s="3">
+        <v>16632</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" s="3">
+        <v>9381</v>
+      </c>
+      <c r="C16" s="3">
+        <v>23884</v>
+      </c>
+      <c r="D16" s="3">
+        <v>16632</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B18" s="3">
+        <v>392363.79881426215</v>
+      </c>
+      <c r="C18" s="3">
+        <v>482670.07181290811</v>
+      </c>
+      <c r="D18" s="3">
+        <v>437516.93531358516</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" s="3">
+        <v>120663.90029492631</v>
+      </c>
+      <c r="C19" s="3">
+        <v>137624.56862494192</v>
+      </c>
+      <c r="D19" s="3">
+        <v>129144.23445993412</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B20" s="3">
+        <v>6113690.5805921648</v>
+      </c>
+      <c r="C20" s="3">
+        <v>7495192.1551600974</v>
+      </c>
+      <c r="D20" s="3">
+        <v>6804441.3678761311</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" s="3">
+        <v>2433146.2881052429</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2910678.5411954471</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2671912.4146503452</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="3">
+        <v>412003.92714285717</v>
+      </c>
+      <c r="C22" s="3">
+        <v>993370.92714285711</v>
+      </c>
+      <c r="D22" s="3">
+        <v>679905.92714285711</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23" s="3">
+        <v>2121892.0299567101</v>
+      </c>
+      <c r="C23" s="3">
+        <v>4828497.67995671</v>
+      </c>
+      <c r="D23" s="3">
+        <v>2979969.0299567101</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1224606.7557142859</v>
+      </c>
+      <c r="C24" s="3">
+        <v>4476294.0835714294</v>
+      </c>
+      <c r="D24" s="3">
+        <v>3045723.5235714288</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B25" s="3">
+        <v>5710857.2175354939</v>
+      </c>
+      <c r="C25" s="3">
+        <v>10344046.119960569</v>
+      </c>
+      <c r="D25" s="3">
+        <v>8222724.7726766029</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B26" s="3">
+        <v>2962518.6551757222</v>
+      </c>
+      <c r="C26" s="3">
+        <v>6691738.2361230711</v>
+      </c>
+      <c r="D26" s="3">
+        <v>5022401.5495779682</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" s="3">
+        <v>5598401.5460612318</v>
+      </c>
+      <c r="C27" s="3">
+        <v>7149365.6769728297</v>
+      </c>
+      <c r="D27" s="3">
+        <v>6373883.6115170307</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="3">
+        <v>630584.52044832578</v>
+      </c>
+      <c r="C28" s="3">
+        <v>711818.5262609612</v>
+      </c>
+      <c r="D28" s="3">
+        <v>671201.52335464349</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B29" s="3">
+        <v>10502777.813854344</v>
+      </c>
+      <c r="C29" s="3">
+        <v>18505173.372092053</v>
+      </c>
+      <c r="D29" s="3">
+        <v>14181241.371901771</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B30" s="3">
+        <v>9381</v>
+      </c>
+      <c r="C30" s="3">
+        <v>23884</v>
+      </c>
+      <c r="D30" s="3">
+        <v>16632</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" s="3">
+        <v>9381</v>
+      </c>
+      <c r="C31" s="3">
+        <v>23884</v>
+      </c>
+      <c r="D31" s="3">
+        <v>16632</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" s="3">
+        <v>2656482.1929747607</v>
+      </c>
+      <c r="C33" s="3">
+        <v>2943069.3142786585</v>
+      </c>
+      <c r="D33" s="3">
+        <v>2799775.7536267098</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="3">
+        <v>306688.60299137124</v>
+      </c>
+      <c r="C34" s="3">
+        <v>379648.48229144717</v>
+      </c>
+      <c r="D34" s="3">
+        <v>343168.54264140921</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" s="3">
+        <v>26761284.026168723</v>
+      </c>
+      <c r="C35" s="3">
+        <v>46433035.9327038</v>
+      </c>
+      <c r="D35" s="3">
+        <v>41637773.839061804</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" s="3">
+        <v>18753556.669676185</v>
+      </c>
+      <c r="C36" s="3">
+        <v>22639629.325349167</v>
+      </c>
+      <c r="D36" s="3">
+        <v>20696592.997512676</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B37" s="3">
+        <v>509826.75</v>
+      </c>
+      <c r="C37" s="3">
+        <v>3527954.75</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1914709.75</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="3">
+        <v>5861116.019480519</v>
+      </c>
+      <c r="C38" s="3">
+        <v>12605808.019480519</v>
+      </c>
+      <c r="D38" s="3">
+        <v>6483873.019480519</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1385172.25</v>
+      </c>
+      <c r="C39" s="3">
+        <v>4312581.805555556</v>
+      </c>
+      <c r="D39" s="3">
+        <v>3079323.8055555555</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="3">
+        <v>19784040.170354191</v>
+      </c>
+      <c r="C40" s="3">
+        <v>32301973.913193736</v>
+      </c>
+      <c r="D40" s="3">
+        <v>26273453.81955174</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41" s="3">
+        <v>9702812.4511031024</v>
+      </c>
+      <c r="C41" s="3">
+        <v>16516294.662331637</v>
+      </c>
+      <c r="D41" s="3">
+        <v>13340000.334495148</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B42" s="3">
+        <v>23865124.694085877</v>
+      </c>
+      <c r="C42" s="3">
+        <v>34333122.980447814</v>
+      </c>
+      <c r="D42" s="3">
+        <v>29099123.837266844</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B43" s="3">
+        <v>2638661.215704733</v>
+      </c>
+      <c r="C43" s="3">
+        <v>3053153.7670242894</v>
+      </c>
+      <c r="D43" s="3">
+        <v>2845907.4913645112</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B44" s="3">
+        <v>37156060.261353977</v>
+      </c>
+      <c r="C44" s="3">
+        <v>69932534.274764165</v>
+      </c>
+      <c r="D44" s="3">
+        <v>55961587.905462384</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45" s="3">
+        <v>10590</v>
+      </c>
+      <c r="C45" s="3">
+        <v>20415</v>
+      </c>
+      <c r="D45" s="3">
+        <v>15503</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B46" s="5">
+        <v>37572</v>
+      </c>
+      <c r="C46" s="3">
+        <v>64922</v>
+      </c>
+      <c r="D46" s="5">
+        <v>51247</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B48" s="3">
+        <v>2954993.5579487886</v>
+      </c>
+      <c r="C48" s="3">
+        <v>3276093.9863089053</v>
+      </c>
+      <c r="D48" s="3">
+        <v>3115543.772128847</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B49" s="3">
+        <v>326795.79728797026</v>
+      </c>
+      <c r="C49" s="3">
+        <v>407700.83987982059</v>
+      </c>
+      <c r="D49" s="3">
+        <v>367248.31858389539</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" s="3">
+        <v>37956384.953797422</v>
+      </c>
+      <c r="C50" s="3">
+        <v>47702504.639027342</v>
+      </c>
+      <c r="D50" s="3">
+        <v>42829444.796412379</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B51" s="3">
+        <v>13377907.078417799</v>
+      </c>
+      <c r="C51" s="3">
+        <v>17284577.589700673</v>
+      </c>
+      <c r="D51" s="3">
+        <v>15331242.334059237</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B52" s="3">
+        <v>509826.75</v>
+      </c>
+      <c r="C52" s="3">
+        <v>3527954.75</v>
+      </c>
+      <c r="D52" s="3">
+        <v>1914709.75</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B53" s="3">
+        <v>5861116.019480519</v>
+      </c>
+      <c r="C53" s="3">
+        <v>12605808.019480519</v>
+      </c>
+      <c r="D53" s="3">
+        <v>6483873.019480519</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B54" s="3">
+        <v>1385172.25</v>
+      </c>
+      <c r="C54" s="3">
+        <v>4312581.805555556</v>
+      </c>
+      <c r="D54" s="3">
+        <v>3079323.8055555555</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B55" s="3">
+        <v>19995920.070162319</v>
+      </c>
+      <c r="C55" s="3">
+        <v>32669449.310947791</v>
+      </c>
+      <c r="D55" s="3">
+        <v>26563131.468332835</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B56" s="3">
+        <v>9730937.841586832</v>
+      </c>
+      <c r="C56" s="3">
+        <v>16565017.908425266</v>
+      </c>
+      <c r="D56" s="3">
+        <v>13378424.652783828</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B57" s="3">
+        <v>24077004.593894005</v>
+      </c>
+      <c r="C57" s="3">
+        <v>34700598.378201872</v>
+      </c>
+      <c r="D57" s="3">
+        <v>29388801.486047938</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B58" s="3">
+        <v>2638661.215704733</v>
+      </c>
+      <c r="C58" s="3">
+        <v>3053153.7670242894</v>
+      </c>
+      <c r="D58" s="3">
+        <v>2845907.4913645112</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B59" s="3">
+        <v>48351161.188982673</v>
+      </c>
+      <c r="C59" s="3">
+        <v>71202002.981087714</v>
+      </c>
+      <c r="D59" s="3">
+        <v>57153258.862812959</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B60" s="3">
+        <v>10590</v>
+      </c>
+      <c r="C60" s="3">
+        <v>20415</v>
+      </c>
+      <c r="D60" s="3">
+        <v>15503</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B61" s="5">
+        <v>37572</v>
+      </c>
+      <c r="C61" s="3">
+        <v>64922</v>
+      </c>
+      <c r="D61" s="5">
+        <v>51247</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>